<commit_message>
Terminado path and query
</commit_message>
<xml_diff>
--- a/API solo GET/Registros.xlsx
+++ b/API solo GET/Registros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Universidad\7mo_Semestre\ModelosDesarrolloWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Universidad\7mo_Semestre\ModelosDesarrolloWeb\API solo GET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692EA688-37FA-461C-A90A-E4C0374DDB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4000C26-85B5-4AD2-92D9-4194C7D02A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{56199526-209F-421B-A59B-221EA2FB9C7B}"/>
   </bookViews>
@@ -255,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,6 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE88BA5-6EDD-4E09-B3D2-6A3732D879E1}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>9.01</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>9.01</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="3">
-        <v>9.01</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1507,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>8.98</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1571,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>8.98</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1603,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>8.98</v>
+        <v>8.07</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1699,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>8.98</v>
+        <v>8.65</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1731,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>8.98</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1812,7 +1813,7 @@
         <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F38">
         <v>8</v>
@@ -1823,7 +1824,7 @@
       <c r="H38" t="s">
         <v>29</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="10">
         <v>1</v>
       </c>
       <c r="J38" s="3">
@@ -2088,5 +2089,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>